<commit_message>
sn: update sch/sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Senegal/2023/sn_sch_sth_impact_2_child_202308.xlsx
+++ b/SCH-STH/Impact assessments/Senegal/2023/sn_sch_sth_impact_2_child_202308.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Senegal\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA239A90-B758-4E9E-9019-2D0258AED9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102A1289-7A86-4115-9F3C-63F59DD259EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -504,12 +504,6 @@
     <t>p_barcodeid</t>
   </si>
   <si>
-    <t>sn_sch_sth_impact_2_child_202308</t>
-  </si>
-  <si>
-    <t>(Août 2023) - 2. SCH/STH – Participant</t>
-  </si>
-  <si>
     <t>p_annes_vecu_village</t>
   </si>
   <si>
@@ -519,12 +513,6 @@
     <t>. &lt;= ${p_age_yrs}</t>
   </si>
   <si>
-    <t>. &gt;= 8 and . &lt;= 14</t>
-  </si>
-  <si>
-    <t>L’âge doit être compris entre 8 et 14 ans</t>
-  </si>
-  <si>
     <t>L'année ne doit pas déppasé l'age de l'enfant</t>
   </si>
   <si>
@@ -537,7 +525,19 @@
     <t>p_pisse_sang_maintenant</t>
   </si>
   <si>
-    <t>14. Est-ce que présentement vous pissez du sang ?</t>
+    <t>(Août 2023) - 2. SCH/STH – Participant V2</t>
+  </si>
+  <si>
+    <t>sn_sch_sth_impact_2_child_202308_v2</t>
+  </si>
+  <si>
+    <t>15. Est-ce que présentement vous pissez du sang ?</t>
+  </si>
+  <si>
+    <t>. &gt;= 5 and . &lt;= 14</t>
+  </si>
+  <si>
+    <t>L’âge doit être compris entre 5 et 14 ans</t>
   </si>
 </sst>
 </file>
@@ -1060,11 +1060,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1083,7 @@
     <col min="12" max="12" width="16.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="16" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1370,10 +1370,10 @@
       <c r="D13" s="10"/>
       <c r="E13" s="8"/>
       <c r="F13" s="31" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="H13" s="30" t="s">
         <v>26</v>
@@ -1438,18 +1438,18 @@
         <v>29</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H16" s="30" t="s">
         <v>26</v>
@@ -1552,10 +1552,10 @@
         <v>27</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="24"/>
@@ -1576,10 +1576,10 @@
         <v>27</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="24"/>
@@ -2299,8 +2299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2320,12 +2320,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
sn: update sch/sth form
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Senegal/2023/sn_sch_sth_impact_2_child_202308.xlsx
+++ b/SCH-STH/Impact assessments/Senegal/2023/sn_sch_sth_impact_2_child_202308.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Senegal\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031041A0-2D83-44D0-9C2A-86DD264DCACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357BF9AB-44D6-4F31-994B-5888305241B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="230">
   <si>
     <t>type</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>La réponse "Non" mettra fin à l'enquête</t>
-  </si>
-  <si>
-    <t>${p_consent} = 'A.donne'</t>
   </si>
   <si>
     <r>
@@ -156,9 +153,6 @@
     <t>Vous venez d'entrer une valeur qui entrainera la fin de l'enquête</t>
   </si>
   <si>
-    <t>${p_consent} = 'A.refuse'</t>
-  </si>
-  <si>
     <t>p_remarks</t>
   </si>
   <si>
@@ -471,9 +465,6 @@
     <t>p_note_thanks</t>
   </si>
   <si>
-    <t>${p_consent} = 'A.donne' and ${p_connait_bilh} = 'Oui'</t>
-  </si>
-  <si>
     <t>Note additionnelle :</t>
   </si>
   <si>
@@ -526,12 +517,6 @@
   </si>
   <si>
     <t>L’âge doit être compris entre 5 et 14 ans</t>
-  </si>
-  <si>
-    <t>(Août 2023) - 2. SCH/STH – Participant V3</t>
-  </si>
-  <si>
-    <t>sn_sch_sth_impact_2_child_202308_v3</t>
   </si>
   <si>
     <t>9. Y a-t-il des toilettes à la concession ?</t>
@@ -747,6 +732,30 @@
   </si>
   <si>
     <t>5. Sélectionnez le code du village</t>
+  </si>
+  <si>
+    <t>(Août 2023) - 2. SCH/STH – Participant V3.2</t>
+  </si>
+  <si>
+    <t>sn_sch_sth_impact_2_child_202308_v3_2</t>
+  </si>
+  <si>
+    <t>p_add_child</t>
+  </si>
+  <si>
+    <t>Voulez-vous vraiment enregistrer un nouvel enfant?</t>
+  </si>
+  <si>
+    <t>${p_add_child} = 'Oui'</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'A.donne' and ${p_add_child} = 'Oui'</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'A.donne' and ${p_connait_bilh} = 'Oui' and ${p_add_child} = 'Oui'</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'A.refuse' and ${p_add_child} = 'Oui'</t>
   </si>
 </sst>
 </file>
@@ -1285,13 +1294,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1357,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="17" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -1359,17 +1368,17 @@
         <v>12</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -1387,7 +1396,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="8"/>
@@ -1409,7 +1418,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="8"/>
@@ -1433,7 +1442,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="8"/>
@@ -1454,10 +1463,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="8"/>
@@ -1470,7 +1479,7 @@
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="18" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1489,13 +1498,13 @@
     </row>
     <row r="8" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="44"/>
@@ -1509,22 +1518,22 @@
       <c r="K8" s="44"/>
       <c r="L8" s="44"/>
     </row>
-    <row r="9" spans="1:13" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D9" s="45"/>
       <c r="E9" s="44"/>
       <c r="F9" s="44"/>
       <c r="G9" s="45"/>
       <c r="H9" s="30" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I9" s="44"/>
       <c r="J9" s="44" t="s">
@@ -1533,22 +1542,22 @@
       <c r="K9" s="44"/>
       <c r="L9" s="44"/>
     </row>
-    <row r="10" spans="1:13" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D10" s="45"/>
       <c r="E10" s="44"/>
       <c r="F10" s="44"/>
       <c r="G10" s="45"/>
       <c r="H10" s="30" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I10" s="44"/>
       <c r="J10" s="44" t="s">
@@ -1557,22 +1566,22 @@
       <c r="K10" s="44"/>
       <c r="L10" s="44"/>
     </row>
-    <row r="11" spans="1:13" s="37" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="45"/>
       <c r="H11" s="30" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I11" s="44"/>
       <c r="J11" s="44" t="s">
@@ -1581,22 +1590,22 @@
       <c r="K11" s="44"/>
       <c r="L11" s="44"/>
     </row>
-    <row r="12" spans="1:13" s="37" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D12" s="45"/>
       <c r="E12" s="44"/>
       <c r="F12" s="44"/>
       <c r="G12" s="45"/>
       <c r="H12" s="30" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I12" s="44"/>
       <c r="J12" s="44" t="s">
@@ -1605,22 +1614,22 @@
       <c r="K12" s="44"/>
       <c r="L12" s="44"/>
     </row>
-    <row r="13" spans="1:13" s="37" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="44"/>
       <c r="F13" s="44"/>
       <c r="G13" s="45"/>
       <c r="H13" s="30" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I13" s="44"/>
       <c r="J13" s="44" t="s">
@@ -1631,20 +1640,20 @@
     </row>
     <row r="14" spans="1:13" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D14" s="47"/>
       <c r="E14" s="48"/>
       <c r="F14" s="48"/>
       <c r="G14" s="47"/>
       <c r="H14" s="30" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I14" s="48"/>
       <c r="J14" s="44" t="s">
@@ -1655,20 +1664,20 @@
     </row>
     <row r="15" spans="1:13" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D15" s="47"/>
       <c r="E15" s="48"/>
       <c r="F15" s="48"/>
       <c r="G15" s="47"/>
       <c r="H15" s="30" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I15" s="48"/>
       <c r="J15" s="44" t="s">
@@ -1679,20 +1688,20 @@
     </row>
     <row r="16" spans="1:13" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D16" s="47"/>
       <c r="E16" s="48"/>
       <c r="F16" s="48"/>
       <c r="G16" s="47"/>
       <c r="H16" s="30" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I16" s="48"/>
       <c r="J16" s="44" t="s">
@@ -1703,20 +1712,20 @@
     </row>
     <row r="17" spans="1:13" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="46" t="s">
         <v>167</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="C17" s="46" t="s">
-        <v>172</v>
       </c>
       <c r="D17" s="47"/>
       <c r="E17" s="48"/>
       <c r="F17" s="48"/>
       <c r="G17" s="47"/>
       <c r="H17" s="30" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I17" s="48"/>
       <c r="J17" s="44" t="s">
@@ -1727,20 +1736,20 @@
     </row>
     <row r="18" spans="1:13" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D18" s="47"/>
       <c r="E18" s="48"/>
       <c r="F18" s="48"/>
       <c r="G18" s="47"/>
       <c r="H18" s="30" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I18" s="48"/>
       <c r="J18" s="44" t="s">
@@ -1765,10 +1774,10 @@
     </row>
     <row r="20" spans="1:13" s="18" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1781,185 +1790,183 @@
       <c r="K20" s="39"/>
       <c r="L20" s="39"/>
     </row>
-    <row r="21" spans="1:13" s="18" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:13" s="18" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+    </row>
+    <row r="22" spans="1:13" s="18" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-    </row>
-    <row r="22" spans="1:13" s="18" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="10"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-    </row>
-    <row r="23" spans="1:13" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:13" s="18" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+    </row>
+    <row r="24" spans="1:13" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B24" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C24" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K23" s="9"/>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="1:13" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="31"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="I24" s="30"/>
+      <c r="H24" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="I24" s="9"/>
       <c r="J24" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="3"/>
-    </row>
-    <row r="25" spans="1:13" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>30</v>
+        <v>145</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="G25" s="29" t="s">
-        <v>158</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="I25" s="8"/>
+        <v>227</v>
+      </c>
+      <c r="I25" s="30"/>
       <c r="J25" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="1:13" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D26" s="10"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="26"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>155</v>
+      </c>
       <c r="H26" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="24"/>
+        <v>227</v>
+      </c>
+      <c r="I26" s="8"/>
       <c r="J26" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-    </row>
-    <row r="27" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
-        <v>116</v>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>115</v>
+        <v>31</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="26"/>
       <c r="H27" s="30" t="s">
-        <v>26</v>
+        <v>227</v>
       </c>
       <c r="I27" s="24"/>
-      <c r="J27" s="39" t="s">
+      <c r="J27" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
     </row>
-    <row r="28" spans="1:13" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
-        <v>29</v>
+    <row r="28" spans="1:13" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>114</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="24"/>
-      <c r="F28" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>152</v>
-      </c>
+      <c r="F28" s="24"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="30" t="s">
-        <v>26</v>
+        <v>227</v>
       </c>
       <c r="I28" s="24"/>
       <c r="J28" s="39" t="s">
@@ -1968,60 +1975,64 @@
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
     </row>
-    <row r="29" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="29"/>
+    <row r="29" spans="1:13" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>147</v>
+      </c>
       <c r="D29" s="10"/>
       <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="30"/>
+      <c r="F29" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>227</v>
+      </c>
       <c r="I29" s="24"/>
-      <c r="J29" s="39"/>
+      <c r="J29" s="39" t="s">
+        <v>13</v>
+      </c>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
     </row>
-    <row r="30" spans="1:13" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>147</v>
-      </c>
+    <row r="30" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="10"/>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="26"/>
-      <c r="H30" s="30" t="s">
-        <v>26</v>
-      </c>
+      <c r="H30" s="30"/>
       <c r="I30" s="24"/>
-      <c r="J30" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="J30" s="39"/>
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
     </row>
-    <row r="31" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
-        <v>27</v>
+    <row r="31" spans="1:13" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>119</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="26"/>
       <c r="H31" s="30" t="s">
-        <v>26</v>
+        <v>227</v>
       </c>
       <c r="I31" s="24"/>
       <c r="J31" s="30" t="s">
@@ -2031,21 +2042,21 @@
       <c r="L31" s="24"/>
     </row>
     <row r="32" spans="1:13" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
-        <v>129</v>
+      <c r="A32" s="39" t="s">
+        <v>26</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
       <c r="G32" s="26"/>
       <c r="H32" s="30" t="s">
-        <v>140</v>
+        <v>227</v>
       </c>
       <c r="I32" s="24"/>
       <c r="J32" s="30" t="s">
@@ -2054,22 +2065,22 @@
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
     </row>
-    <row r="33" spans="1:12" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
-        <v>27</v>
+    <row r="33" spans="1:12" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>127</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
       <c r="G33" s="26"/>
       <c r="H33" s="30" t="s">
-        <v>26</v>
+        <v>228</v>
       </c>
       <c r="I33" s="24"/>
       <c r="J33" s="30" t="s">
@@ -2078,22 +2089,22 @@
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
     </row>
-    <row r="34" spans="1:12" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
       <c r="G34" s="26"/>
       <c r="H34" s="30" t="s">
-        <v>26</v>
+        <v>227</v>
       </c>
       <c r="I34" s="24"/>
       <c r="J34" s="30" t="s">
@@ -2102,88 +2113,98 @@
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
     </row>
-    <row r="35" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
+    <row r="35" spans="1:12" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="I35" s="24"/>
+      <c r="J35" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+    </row>
+    <row r="36" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B36" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="40" t="s">
         <v>33</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="40" t="s">
-        <v>141</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="12"/>
-      <c r="H36" s="24"/>
+      <c r="H36" s="31" t="s">
+        <v>229</v>
+      </c>
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
     </row>
-    <row r="37" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="43" t="s">
-        <v>20</v>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>139</v>
+        <v>34</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="12"/>
-      <c r="H37" s="30" t="s">
-        <v>26</v>
-      </c>
+      <c r="H37" s="24"/>
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
     </row>
-    <row r="38" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="25"/>
+    <row r="38" spans="1:12" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>132</v>
+      </c>
       <c r="D38" s="12"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="12"/>
-      <c r="H38" s="24"/>
+      <c r="H38" s="30" t="s">
+        <v>227</v>
+      </c>
       <c r="I38" s="11"/>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
       <c r="L38" s="11"/>
     </row>
     <row r="39" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
+      <c r="A39" s="22" t="s">
+        <v>183</v>
+      </c>
       <c r="B39" s="22"/>
       <c r="C39" s="25"/>
       <c r="D39" s="12"/>
@@ -2196,13 +2217,9 @@
       <c r="K39" s="11"/>
       <c r="L39" s="11"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>38</v>
-      </c>
+    <row r="40" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
       <c r="C40" s="25"/>
       <c r="D40" s="12"/>
       <c r="E40" s="11"/>
@@ -2215,11 +2232,11 @@
       <c r="L40" s="11"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>39</v>
+      <c r="A41" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="12"/>
@@ -2231,6 +2248,24 @@
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
       <c r="L41" s="11"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2257,7 +2292,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
@@ -2266,16 +2301,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2286,25 +2321,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>46</v>
-      </c>
       <c r="C4" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="33"/>
     </row>
@@ -2316,25 +2351,25 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="C7" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D7" s="35"/>
     </row>
@@ -2346,25 +2381,25 @@
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D9" s="33"/>
     </row>
     <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="D10" s="33"/>
     </row>
@@ -2376,73 +2411,73 @@
     </row>
     <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" s="33"/>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D14" s="33"/>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D15" s="33"/>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" s="33"/>
     </row>
     <row r="17" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17" s="33"/>
     </row>
@@ -2454,37 +2489,37 @@
     </row>
     <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="D19" s="33"/>
     </row>
     <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D20" s="33"/>
     </row>
     <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="33"/>
     </row>
@@ -2496,247 +2531,247 @@
     </row>
     <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="D23" s="33"/>
     </row>
     <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D26" s="33"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>79</v>
-      </c>
       <c r="C27" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D27" s="33"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D28" s="33"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D29" s="33"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D30" s="33"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D31" s="33"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D32" s="33"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D38" s="27"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D39" s="27"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D40" s="27"/>
     </row>
     <row r="42" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B42" s="42" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D42" s="37"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B43" s="42" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B44" s="42" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D44" s="37"/>
     </row>
@@ -2747,49 +2782,49 @@
     </row>
     <row r="46" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C46" s="42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D46" s="37"/>
     </row>
     <row r="47" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="B47" s="42" t="s">
-        <v>132</v>
-      </c>
       <c r="C47" s="37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D47" s="37"/>
     </row>
     <row r="48" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D48" s="37"/>
     </row>
     <row r="49" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D49" s="37"/>
     </row>
@@ -2800,214 +2835,214 @@
     </row>
     <row r="51" spans="1:4" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B51" s="44" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C51" s="45" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:4" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B52" s="44" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C52" s="45" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D52" s="11"/>
     </row>
     <row r="53" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B53" s="44" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C53" s="45" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D53" s="11"/>
     </row>
     <row r="54" spans="1:4" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B54" s="44" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C54" s="45" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D54" s="11"/>
     </row>
     <row r="55" spans="1:4" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="B55" s="44" t="s">
-        <v>194</v>
-      </c>
       <c r="C55" s="45" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D55" s="11"/>
     </row>
     <row r="57" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C57" s="45" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D57" s="11"/>
     </row>
     <row r="58" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C58" s="45" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D58" s="11"/>
     </row>
     <row r="59" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C59" s="45" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D59" s="11"/>
     </row>
     <row r="60" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="44" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C60" s="45" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D60" s="11"/>
     </row>
     <row r="62" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B62" s="44" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C62" s="45" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D62" s="11"/>
     </row>
     <row r="63" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C63" s="45" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C64" s="45" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B65" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="B65" s="30" t="s">
-        <v>206</v>
-      </c>
       <c r="C65" s="45" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D65" s="11"/>
     </row>
     <row r="66" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C66" s="45" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D66" s="11"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>204</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3021,7 +3056,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3032,24 +3067,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>160</v>
+        <v>223</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>